<commit_message>
added new search engine feature
</commit_message>
<xml_diff>
--- a/database_dum_exc.xlsx
+++ b/database_dum_exc.xlsx
@@ -433,59 +433,59 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Kontrak Asana</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AHM</t>
+          <t>abadi ehe</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>16-06-2020 21:00:00</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>16-06-2020 22:46:00</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>E:/16719147_Arsyi Adlani_Summary.pdf</t>
+          <t>E:/16719147 Arsyi Adlani Introductory Paragraph.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Kontrak Asana</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AHM</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>16-06-2020 21:00:00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>16-06-2020 22:46:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">

</xml_diff>